<commit_message>
merge new SSR/TR and refactoring
</commit_message>
<xml_diff>
--- a/TR/TR.xlsx
+++ b/TR/TR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bo/Documents/projects/DomainModelExtractor/TR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FEF7B5-7F9E-A748-846B-CCB5DF29595C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B51EA64-8916-0542-8437-4689A0B8BE49}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15620" yWindow="1020" windowWidth="13060" windowHeight="16540" xr2:uid="{5C7C09FE-FFCB-6240-8A81-2E4E06E0E700}"/>
+    <workbookView xWindow="9060" yWindow="920" windowWidth="19740" windowHeight="16540" xr2:uid="{5C7C09FE-FFCB-6240-8A81-2E4E06E0E700}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
   <si>
     <t>TR1</t>
   </si>
@@ -51,23 +51,152 @@
     <t>add_behavior</t>
   </si>
   <si>
-    <t>SVDO</t>
-  </si>
-  <si>
     <t>actor=B, target=C, action=A</t>
+  </si>
+  <si>
+    <t>TR2</t>
+  </si>
+  <si>
+    <t>actor=B, action=C</t>
+  </si>
+  <si>
+    <t>actor=B, target=D, action=C</t>
+  </si>
+  <si>
+    <t>actor=B, action=A</t>
+  </si>
+  <si>
+    <t>SV</t>
+  </si>
+  <si>
+    <t>TR3</t>
+  </si>
+  <si>
+    <t>TR4</t>
+  </si>
+  <si>
+    <t>TR5</t>
+  </si>
+  <si>
+    <t>add_entity_attribute</t>
+  </si>
+  <si>
+    <t>TR6</t>
+  </si>
+  <si>
+    <t>actor=B, action=AC</t>
+  </si>
+  <si>
+    <t>TR7</t>
+  </si>
+  <si>
+    <t>actor=B, action=AC, target=D</t>
+  </si>
+  <si>
+    <t>entity_name=B, attr_name=A</t>
+  </si>
+  <si>
+    <t>SVObj</t>
+  </si>
+  <si>
+    <t>SVObl</t>
+  </si>
+  <si>
+    <t>SVCcO</t>
+  </si>
+  <si>
+    <t>SVCc</t>
+  </si>
+  <si>
+    <t>SVpO</t>
+  </si>
+  <si>
+    <t>SVp</t>
+  </si>
+  <si>
+    <t>Poss</t>
+  </si>
+  <si>
+    <t>TR8</t>
+  </si>
+  <si>
+    <t>actor=C, target=B, action=A</t>
+  </si>
+  <si>
+    <t>VOToInf</t>
+  </si>
+  <si>
+    <t>TR9</t>
+  </si>
+  <si>
+    <t>TR10</t>
+  </si>
+  <si>
+    <t>SVThatClause</t>
+  </si>
+  <si>
+    <t>actor=B, target=E, action=A</t>
+  </si>
+  <si>
+    <t>TR11</t>
+  </si>
+  <si>
+    <t>SVOblWith</t>
+  </si>
+  <si>
+    <t>SVByVO</t>
+  </si>
+  <si>
+    <t>SVByV</t>
+  </si>
+  <si>
+    <t>TR12</t>
+  </si>
+  <si>
+    <t>TR13</t>
+  </si>
+  <si>
+    <t>OPassVS</t>
+  </si>
+  <si>
+    <t>add_relation</t>
+  </si>
+  <si>
+    <t>TR14</t>
+  </si>
+  <si>
+    <t>source=B, dest=C, msg="supported_by", ass_type="association"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -90,8 +219,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,20 +538,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39E7213-EEEB-7B4F-8631-8D0922B73947}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:Z15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" customWidth="1"/>
-    <col min="4" max="4" width="41" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="57.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -433,18 +565,222 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
merge and test new SSRs for OCO and VCV cases
</commit_message>
<xml_diff>
--- a/TR/TR.xlsx
+++ b/TR/TR.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bo/Documents/projects/DomainModelExtractor-test/TR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bo/Documents/projects/DomainModelExtractor/TR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331A6D6F-542B-1948-BDCF-333D17E310C5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C3A68A-F0F6-A847-B4D5-797AB9AB9669}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9060" yWindow="540" windowWidth="19740" windowHeight="16540" xr2:uid="{5C7C09FE-FFCB-6240-8A81-2E4E06E0E700}"/>
+    <workbookView xWindow="13440" yWindow="960" windowWidth="19740" windowHeight="16540" xr2:uid="{5C7C09FE-FFCB-6240-8A81-2E4E06E0E700}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="67">
   <si>
     <t>TR1</t>
   </si>
@@ -187,13 +187,58 @@
   </si>
   <si>
     <t>SVCVO</t>
+  </si>
+  <si>
+    <t>TR18</t>
+  </si>
+  <si>
+    <t>TR19</t>
+  </si>
+  <si>
+    <t>actor=B, target=E, action=C</t>
+  </si>
+  <si>
+    <t>TR20</t>
+  </si>
+  <si>
+    <t>actor=B, target=E, action=D</t>
+  </si>
+  <si>
+    <t>SVOCO</t>
+  </si>
+  <si>
+    <t>TR21</t>
+  </si>
+  <si>
+    <t>TR22</t>
+  </si>
+  <si>
+    <t>SVVO1Comma</t>
+  </si>
+  <si>
+    <t>actor=B, target=D, action=A</t>
+  </si>
+  <si>
+    <t>SVVOMultiComma</t>
+  </si>
+  <si>
+    <t>TR23</t>
+  </si>
+  <si>
+    <t>TR24</t>
+  </si>
+  <si>
+    <t>SVOOComma</t>
+  </si>
+  <si>
+    <t>TR25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -225,6 +270,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -246,11 +297,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39E7213-EEEB-7B4F-8631-8D0922B73947}">
-  <dimension ref="A1:Z19"/>
+  <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -853,8 +905,120 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="3"/>
-      <c r="C19" s="2"/>
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>